<commit_message>
Updated receptacle tests for demo. All pass!
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/receptacle_tests_demo.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/receptacle_tests_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF38CA71-4B60-4F1E-A1E7-E0CD1AEFAEAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011B6AC4-3725-4018-92CD-820E5EFBD892}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="9" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="120">
   <si>
     <t>pass</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>multiplier_schedule_name</t>
+  </si>
+  <si>
+    <t>expected_rule_outcome</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="202">
+  <dxfs count="82">
     <dxf>
       <fill>
         <patternFill>
@@ -787,139 +790,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -955,111 +825,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1095,637 +860,35 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2385,15 +1548,15 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF23" sqref="AF23"/>
+      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" style="9" bestFit="1" customWidth="1"/>
@@ -2585,8 +1748,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>54</v>
+      <c r="A6" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -3690,7 +2853,7 @@
         <v>45</v>
       </c>
       <c r="E50" s="11"/>
-      <c r="K50" s="1">
+      <c r="J50" s="1">
         <v>3</v>
       </c>
     </row>
@@ -3708,7 +2871,7 @@
         <v>93</v>
       </c>
       <c r="E51" s="11"/>
-      <c r="K51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4019,298 +3182,303 @@
       <c r="E71" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A59:E64 A65:B69 A5:E45">
-    <cfRule type="expression" dxfId="201" priority="255">
+  <conditionalFormatting sqref="A59:E64 A65:B69 A5:E5 A7:E45 B6:E6">
+    <cfRule type="expression" dxfId="81" priority="260">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:D30">
-    <cfRule type="expression" dxfId="200" priority="219">
+    <cfRule type="expression" dxfId="80" priority="224">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E31">
-    <cfRule type="expression" dxfId="199" priority="218">
+    <cfRule type="expression" dxfId="79" priority="223">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:E51 A59:E60 A61:D61 E61:E64 A52:B56">
-    <cfRule type="expression" dxfId="198" priority="211">
+    <cfRule type="expression" dxfId="78" priority="216">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:M38 F10:M20">
-    <cfRule type="expression" dxfId="197" priority="210">
+    <cfRule type="expression" dxfId="77" priority="215">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:M64 F24:M29 F39:M51">
-    <cfRule type="expression" dxfId="196" priority="209">
+    <cfRule type="expression" dxfId="76" priority="214">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:M23">
-    <cfRule type="expression" dxfId="195" priority="197">
+    <cfRule type="expression" dxfId="75" priority="202">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:M22">
-    <cfRule type="expression" dxfId="194" priority="208">
+    <cfRule type="expression" dxfId="74" priority="213">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:M51">
-    <cfRule type="expression" dxfId="193" priority="201">
+    <cfRule type="expression" dxfId="73" priority="206">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:M34 F59:M61 F36:M40 F42:M51">
-    <cfRule type="expression" dxfId="192" priority="205">
+    <cfRule type="expression" dxfId="72" priority="210">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:M9">
-    <cfRule type="expression" dxfId="191" priority="206">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F64:M64 F38:M38 F46:M47 F50:M51 F59:M61">
-    <cfRule type="expression" dxfId="190" priority="204">
+    <cfRule type="expression" dxfId="71" priority="211">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F64:M64 F38:M38 F46:M47 F59:M61 F50:M51">
+    <cfRule type="expression" dxfId="70" priority="209">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:M64">
-    <cfRule type="expression" dxfId="189" priority="203">
+    <cfRule type="expression" dxfId="69" priority="208">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:M49">
-    <cfRule type="expression" dxfId="188" priority="202">
+    <cfRule type="expression" dxfId="68" priority="207">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:M35 F38:M38 F41:M41">
-    <cfRule type="expression" dxfId="187" priority="198">
+    <cfRule type="expression" dxfId="67" priority="203">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:E45">
-    <cfRule type="expression" dxfId="186" priority="196">
+    <cfRule type="expression" dxfId="66" priority="201">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:D45">
-    <cfRule type="expression" dxfId="185" priority="195">
+    <cfRule type="expression" dxfId="65" priority="200">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E45">
-    <cfRule type="expression" dxfId="184" priority="194">
+    <cfRule type="expression" dxfId="64" priority="199">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:M45">
-    <cfRule type="expression" dxfId="183" priority="193">
+    <cfRule type="expression" dxfId="63" priority="198">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:E54 C55 E55">
-    <cfRule type="expression" dxfId="182" priority="192">
+    <cfRule type="expression" dxfId="62" priority="197">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:M55">
-    <cfRule type="expression" dxfId="181" priority="191">
+    <cfRule type="expression" dxfId="61" priority="196">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:M53 F55:M55">
-    <cfRule type="expression" dxfId="180" priority="190">
+    <cfRule type="expression" dxfId="60" priority="195">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:M54">
-    <cfRule type="expression" dxfId="179" priority="189">
+    <cfRule type="expression" dxfId="59" priority="194">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:E54 C55 E55">
-    <cfRule type="expression" dxfId="178" priority="188">
+    <cfRule type="expression" dxfId="58" priority="193">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="177" priority="187">
+    <cfRule type="expression" dxfId="57" priority="192">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="expression" dxfId="176" priority="186">
+    <cfRule type="expression" dxfId="56" priority="191">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:M55">
-    <cfRule type="expression" dxfId="175" priority="185">
+    <cfRule type="expression" dxfId="55" priority="190">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:E67 C68 E68">
-    <cfRule type="expression" dxfId="174" priority="184">
+    <cfRule type="expression" dxfId="54" priority="189">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:M68">
-    <cfRule type="expression" dxfId="173" priority="183">
+    <cfRule type="expression" dxfId="53" priority="188">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:M66 F68:M68">
-    <cfRule type="expression" dxfId="172" priority="182">
+    <cfRule type="expression" dxfId="52" priority="187">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67:M67">
-    <cfRule type="expression" dxfId="171" priority="181">
+    <cfRule type="expression" dxfId="51" priority="186">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:E67 C68 E68">
-    <cfRule type="expression" dxfId="170" priority="180">
+    <cfRule type="expression" dxfId="50" priority="185">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="169" priority="179">
+    <cfRule type="expression" dxfId="49" priority="184">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="168" priority="178">
+    <cfRule type="expression" dxfId="48" priority="183">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:M68">
-    <cfRule type="expression" dxfId="167" priority="177">
+    <cfRule type="expression" dxfId="47" priority="182">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:E58 E56">
-    <cfRule type="expression" dxfId="166" priority="176">
+    <cfRule type="expression" dxfId="46" priority="181">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:M58">
-    <cfRule type="expression" dxfId="165" priority="175">
+    <cfRule type="expression" dxfId="45" priority="180">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:M58">
-    <cfRule type="expression" dxfId="164" priority="174">
+    <cfRule type="expression" dxfId="44" priority="179">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:E58 E56">
-    <cfRule type="expression" dxfId="163" priority="173">
+    <cfRule type="expression" dxfId="43" priority="178">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:D58">
-    <cfRule type="expression" dxfId="162" priority="172">
+    <cfRule type="expression" dxfId="42" priority="177">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E58">
-    <cfRule type="expression" dxfId="161" priority="171">
+    <cfRule type="expression" dxfId="41" priority="176">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:M58">
-    <cfRule type="expression" dxfId="160" priority="170">
+    <cfRule type="expression" dxfId="40" priority="175">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:E71 E69">
-    <cfRule type="expression" dxfId="159" priority="169">
+    <cfRule type="expression" dxfId="39" priority="174">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69:M71">
-    <cfRule type="expression" dxfId="158" priority="168">
+    <cfRule type="expression" dxfId="38" priority="173">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69:M71">
-    <cfRule type="expression" dxfId="157" priority="167">
+    <cfRule type="expression" dxfId="37" priority="172">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:E71 E69">
-    <cfRule type="expression" dxfId="156" priority="166">
+    <cfRule type="expression" dxfId="36" priority="171">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:D71">
-    <cfRule type="expression" dxfId="155" priority="165">
+    <cfRule type="expression" dxfId="35" priority="170">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:E71">
-    <cfRule type="expression" dxfId="154" priority="164">
+    <cfRule type="expression" dxfId="34" priority="169">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69:M71">
-    <cfRule type="expression" dxfId="153" priority="163">
+    <cfRule type="expression" dxfId="33" priority="168">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:D43">
-    <cfRule type="expression" dxfId="61" priority="44">
+    <cfRule type="expression" dxfId="32" priority="49">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="60" priority="43">
+    <cfRule type="expression" dxfId="31" priority="48">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="59" priority="42">
+    <cfRule type="expression" dxfId="30" priority="47">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:D69">
-    <cfRule type="expression" dxfId="58" priority="41">
+    <cfRule type="expression" dxfId="29" priority="46">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:D69">
-    <cfRule type="expression" dxfId="57" priority="40">
+    <cfRule type="expression" dxfId="28" priority="45">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="41" priority="24">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="40" priority="23">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="39" priority="22">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="38" priority="21">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="37" priority="20">
+    <cfRule type="expression" dxfId="23" priority="25">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5466,77 +4634,77 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A41:D52 A24:C24 A5:D20 B53:B56">
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:D36 B37:B40">
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="21" priority="19">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E20 E41:E52">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E36">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="19" priority="16">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:D21 A22:C23 D22:D24">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="18" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:E22">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E24">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40 C40">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:A39 D38:D40 C38:C39 C37:D37">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:E38">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E40">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56 C56">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A55 D54:D56 C54:C55 C53:D53">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E54">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7017,17 +6185,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:D22 A37:D50">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:D34 A35:B36">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D36">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>